<commit_message>
Added View Details when clicking books.
</commit_message>
<xml_diff>
--- a/app/models/books.xlsx
+++ b/app/models/books.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28919"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nationalueduph-my.sharepoint.com/personal/puebloas_students_nu-moa_edu_ph/Documents/Microsoft Teams Chat Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Documents\flask_book_recommender\app\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{566B4A46-9DB4-4359-9ABB-63517913552D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C38EF86-4BEB-41BC-9BD5-4A41DE9F5A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5EE09A01-9BB5-4966-964D-6C13950E5F9C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{5EE09A01-9BB5-4966-964D-6C13950E5F9C}"/>
   </bookViews>
   <sheets>
     <sheet name="book" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="168">
   <si>
     <t>Title</t>
   </si>
@@ -507,13 +507,61 @@
   </si>
   <si>
     <t>https://upload.wikimedia.org/wikipedia/en/b/bb/Fifty_Shades_Darker_book_cover.jpg</t>
+  </si>
+  <si>
+    <t>I knew we were both in mortal danger. Still, in that instant, I felt well. Whole. I could feel my heart racing in my chest, the blood pulsing hot and fast through my veins again. My lungs filled deep with the sweet scent that came off his skin. It was like there had never been any hole in my chest. I was perfect - not healed, but as if there had never been a wound in the first place.
+I FELT LIKE I WAS TRAPPED IN ONE OF THOSE TERRIFYING NIGHTMARES, the one where you have to run, run till your lungs burst, but you can't make your body move fast enough.... But this was no dream, and, unlike the nightmare, I wasn't running for my life; I was racing to save something infinitely more precious. My own life meant little to me today.
+FOR BELLA SWAN THERE IS ONE THING more important than life itself: Edward Cullen. But being in love with a vampire is even more dangerous than Bella could ever have imagined. Edward has already rescued Bella from the clutches of one evil vampire, but now, as their daring relationship threatens all that is near and dear to them, they realize their troubles may be just beginning....
+LEGIONS OF READERS ENTRANCED BY THE New York Times bestseller Twilight are hungry for the continuing story of star-crossed lovers Bell and Edward. In New Moon, Stephanie Meyer delivers another irresistible combination of romance and suspense with a supernatural spin. passionate, riveting, and full of surprising twists and turns, this vampire love saga is well on its way to literary immortality.</t>
+  </si>
+  <si>
+    <t>Jeff Winston was 43 and trapped in a tepid marriage and a dead-end job, waiting for that time when he could be truly happy, when he died.
+And when he woke and he was 18 again, with all his memories of the next 25 years intact. He could live his life again, avoiding the mistakes, making money from his knowledge of the future, seeking happiness.
+Until he dies at 43 and wakes up back in college again...</t>
+  </si>
+  <si>
+    <t>The inventor of the world's first clock is punished for trying to measure God's greatest gift. He is banished to a cave for centuries and forced to listen to the voices of all who come after him seeking more days, more years. Eventually, with his soul nearly broken, Father Time is granted his freedom, along with a magical hourglass and a mission: a chance to redeem himself by teaching two earthly people the true meaning of time.
+He returns to our world - now dominated by the hour-counting he so innocently began - and commences a journey with two unlikely partners: one a teenage girl who is about to give up on life, the other a wealthy old businessman who wants to live forever. To save himself, he must save them both. And stop the world to do so.</t>
+  </si>
+  <si>
+    <t>Combining magic, mysticism, wisdom, and wonder into an inspiring tale of self-discovery, The Alchemist has become a modern classic, selling millions of copies around the world and transforming the lives of countless readers across generations.
+Paulo Coelho's masterpiece tells the mystical story of Santiago, an Andalusian shepherd boy who yearns to travel in search of a worldly treasure. His quest will lead him to riches far different—and far more satisfying—than he ever imagined. Santiago's journey teaches us about the essential wisdom of listening to our hearts, recognizing opportunity and learning to read the omens strewn along life's path, and, most importantly, following our dreams.</t>
+  </si>
+  <si>
+    <t>A masterpiece of rebellion and imprisonment where war is peace freedom is slavery and Big Brother is watching. Thought Police, Big Brother, Orwellian - these words have entered our vocabulary because of George Orwell's classic dystopian novel 1984. The story of one man's Nightmare Odyssey as he pursues a forbidden love affair through a world ruled by warring states and a power structure that controls not only information but also individual thought and memory 1984 is a prophetic haunting tale More relevant than ever before 1984 exposes the worst crimes imaginable the destruction of truth freedom and individuality. With a foreword by Thomas Pynchon. This beautiful paperback edition features deckled edges and french flaps a perfect gift for any occasion</t>
+  </si>
+  <si>
+    <t>Aldous Huxley's profoundly important classic of world literature, Brave New World is a searching vision of an unequal, technologically-advanced future where humans are genetically bred, socially indoctrinated, and pharmaceutically anesthetized to passively uphold an authoritarian ruling order–all at the cost of our freedom, full humanity, and perhaps also our souls. “A genius [who] who spent his life decrying the onward march of the Machine” (The New Yorker), Huxley was a man of incomparable talents: equally an artist, a spiritual seeker, and one of history’s keenest observers of human nature and civilization. Brave New World, his masterpiece, has enthralled and terrified millions of readers, and retains its urgent relevance to this day as both a warning to be heeded as we head into tomorrow and as thought-provoking, satisfying work of literature. Written in the shadow of the rise of fascism during the 1930s, Brave New Worldd likewise speaks to a 21st-century world dominated by mass-entertainment, technology, medicine and pharmaceuticals, the arts of persuasion, and the hidden influence of elites.
+"Aldous Huxley is the greatest 20th century writer in English." —Chicago Tribune</t>
+  </si>
+  <si>
+    <t>At the age of twelve, Jonas, a young boy from a seemingly utopian, futuristic world, is singled out to receive special training from The Giver, who alone holds the memories of the true joys and pain of life.</t>
+  </si>
+  <si>
+    <t>When Nora Seed finds herself in the Midnight Library, she has a chance to make things right. Up until now, her life has been full of misery and regret. She feels she has let everyone down, including herself. But things are about to change.
+The books in the Midnight Library enable Nora to live as if she had done things differently. With the help of an old friend, she can now undo every one of her regrets as she tries to work out her perfect life. But things aren't always what she imagined they'd be, and soon her choices place the library and herself in extreme danger.
+Before time runs out, she must answer the ultimate question: what is the best way to live?</t>
+  </si>
+  <si>
+    <t>The circus arrives without warning. No announcements precede it. It is simply there, when yesterday it was not. Within the black-and-white striped canvas tents is an utterly unique experience full of breathtaking amazements. It is called Le Cirque des Rêves, and it is only open at night.
+But behind the scenes, a fierce competition is underway—a duel between two young magicians, Celia and Marco, who have been trained since childhood expressly for this purpose by their mercurial instructors. Unbeknownst to them, this is a game in which only one can be left standing, and the circus is but the stage for a remarkable battle of imagination and will. Despite themselves, however, Celia and Marco tumble headfirst into love—a deep, magical love that makes the lights flicker and the room grow warm whenever they so much as brush hands.
+True love or not, the game must play out, and the fates of everyone involved, from the cast of extraordinary circus performers to the patrons, hang in the balance, suspended as precariously as the daring acrobats overhead.
+Written in rich, seductive prose, this spell-casting novel is a feast for the senses and the heart.</t>
+  </si>
+  <si>
+    <t>In the house of Helios, god of the sun and mightiest of the Titans, a daughter is born. But Circe is a strange child--neither powerful like her father nor viciously alluring like her mother. Turning to the world of mortals for companionship, she discovers that she does possess power: the power of witchcraft, which can transform rivals into monsters and menace the gods themselves.
+Threatened, Zeus banishes her to a deserted island, where she hones her occult craft, tames wild beasts, and crosses paths with many of the most famous figures in all of mythology, including the Minotaur, Daedalus and his doomed son Icarus, the murderous Medea, and, of course, wily Odysseus.
+But there is danger, too, for a woman who stands alone, and Circe unwittingly draws the wrath of both men and gods, ultimately finding herself pitted against one of the most terrifying and vengeful of the Olympians. To protect what she loves most, Circe must summon all her strength and choose, once and for all, whether she belongs with the gods she is born from or with the mortals she has come to love.</t>
+  </si>
+  <si>
+    <t>Summary</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -922,22 +970,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB145E0-DB29-4C38-857E-07BD615AE8C1}">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="3" width="45.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.140625" customWidth="1"/>
-    <col min="5" max="5" width="136.28515625" customWidth="1"/>
+    <col min="5" max="5" width="175" customWidth="1"/>
+    <col min="6" max="6" width="53.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="24.75" customHeight="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -953,8 +1002,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -970,8 +1022,11 @@
       <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="225" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -987,8 +1042,11 @@
       <c r="E3" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="210" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1004,8 +1062,11 @@
       <c r="E4" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="210" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>1984</v>
       </c>
@@ -1021,8 +1082,11 @@
       <c r="E5" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="360" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1038,8 +1102,11 @@
       <c r="E6" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1055,8 +1122,11 @@
       <c r="E7" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="225" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1072,8 +1142,11 @@
       <c r="E8" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="360" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -1089,8 +1162,11 @@
       <c r="E9" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" s="8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="345" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1106,8 +1182,11 @@
       <c r="E10" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" s="8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -1124,7 +1203,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>48</v>
       </c>
@@ -1141,7 +1220,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -1158,7 +1237,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -1175,7 +1254,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -1192,7 +1271,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -1209,7 +1288,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -1226,7 +1305,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>76</v>
       </c>
@@ -1243,7 +1322,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>80</v>
       </c>
@@ -1260,7 +1339,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>84</v>
       </c>
@@ -1277,7 +1356,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>87</v>
       </c>
@@ -1294,7 +1373,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>91</v>
       </c>
@@ -1311,7 +1390,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>91</v>
       </c>
@@ -1328,7 +1407,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>94</v>
       </c>
@@ -1345,7 +1424,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>98</v>
       </c>
@@ -1361,8 +1440,11 @@
       <c r="E25" s="3" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>100</v>
       </c>
@@ -1379,7 +1461,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="29.25">
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>102</v>
       </c>
@@ -1396,7 +1478,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>105</v>
       </c>
@@ -1413,7 +1495,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>109</v>
       </c>
@@ -1430,7 +1512,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>111</v>
       </c>
@@ -1447,7 +1529,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>113</v>
       </c>
@@ -1464,7 +1546,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>115</v>
       </c>
@@ -1481,7 +1563,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>117</v>
       </c>
@@ -1498,7 +1580,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>119</v>
       </c>
@@ -1515,7 +1597,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>121</v>
       </c>
@@ -1532,7 +1614,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>123</v>
       </c>
@@ -1549,7 +1631,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>125</v>
       </c>
@@ -1566,7 +1648,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>127</v>
       </c>
@@ -1583,7 +1665,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>129</v>
       </c>
@@ -1600,7 +1682,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>131</v>
       </c>
@@ -1617,7 +1699,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>133</v>
       </c>
@@ -1634,7 +1716,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>135</v>
       </c>
@@ -1651,7 +1733,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>137</v>
       </c>
@@ -1668,7 +1750,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>139</v>
       </c>
@@ -1685,7 +1767,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>141</v>
       </c>
@@ -1702,7 +1784,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>143</v>
       </c>
@@ -1719,7 +1801,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>145</v>
       </c>
@@ -1736,7 +1818,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>149</v>
       </c>
@@ -1753,7 +1835,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>153</v>
       </c>
@@ -1770,7 +1852,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>155</v>
       </c>

</xml_diff>